<commit_message>
fix: intercept pred/link actions in scenario mode (ADD_PRED, REMOVE_PRED, ADD_SUC, REMOVE_SUC, UPDATE_PRED)
</commit_message>
<xml_diff>
--- a/Analisis Programa Montec.xlsx
+++ b/Analisis Programa Montec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deivy\OneDrive - Universidad Adolfo Ibanez\Escritorio\Informe Mensual\Informe Montec\Código\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2523BAB3-C3F7-4173-B430-621778AAC45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0DD32C-C6FB-4E6B-97F9-6A9538FD1471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E974F50D-46C4-4847-8353-1A2E4AE2E7D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E974F50D-46C4-4847-8353-1A2E4AE2E7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Programa Enero" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="89">
   <si>
     <t>ID255 (1854 m)</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>FECHA PREVISTA LIBERACIÓN TOTAL</t>
+  </si>
+  <si>
+    <t>Remanente 31-01-2026</t>
   </si>
 </sst>
 </file>
@@ -757,8 +760,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35:Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,7 +772,7 @@
     <col min="11" max="11" width="10.90625" style="1"/>
     <col min="12" max="12" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.453125" style="1" customWidth="1"/>
-    <col min="14" max="16" width="10.90625" style="1"/>
+    <col min="14" max="17" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.35">
@@ -789,6 +792,7 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
+      <c r="Q1"/>
     </row>
     <row r="2" spans="2:18" ht="58" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
@@ -835,6 +839,9 @@
       </c>
       <c r="P2" s="14" t="s">
         <v>86</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
@@ -859,6 +866,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="15"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
@@ -883,6 +891,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
       <c r="R4" s="15"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
@@ -907,6 +916,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
@@ -931,6 +941,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.35">
@@ -955,6 +966,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
@@ -1002,8 +1014,11 @@
         <v>470</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ref="P8:P48" si="1">+O8*N8</f>
-        <v>281.38900000000001</v>
+        <f>+O8-Q8</f>
+        <v>313.96000000000004</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>156.03999999999996</v>
       </c>
       <c r="R8" s="15"/>
     </row>
@@ -1052,8 +1067,11 @@
         <v>65</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="1"/>
-        <v>34.683999999999997</v>
+        <f t="shared" ref="P9:P48" si="1">+O9-Q9</f>
+        <v>45.5</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>19.5</v>
       </c>
       <c r="R9" s="15"/>
     </row>
@@ -1079,6 +1097,7 @@
       <c r="N10" s="8"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
       <c r="R10" s="15"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.35">
@@ -1127,7 +1146,10 @@
       </c>
       <c r="P11" s="2">
         <f t="shared" si="1"/>
-        <v>403.27499999999998</v>
+        <v>451.25</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>23.75</v>
       </c>
       <c r="R11" s="15"/>
     </row>
@@ -1177,7 +1199,10 @@
       </c>
       <c r="P12" s="2">
         <f t="shared" si="1"/>
-        <v>67.69</v>
+        <v>75.754000000000005</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>64.245999999999995</v>
       </c>
       <c r="R12" s="15"/>
     </row>
@@ -1227,7 +1252,10 @@
       </c>
       <c r="P13" s="2">
         <f t="shared" si="1"/>
-        <v>473.82</v>
+        <v>530.22</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>69.779999999999973</v>
       </c>
       <c r="R13" s="15"/>
     </row>
@@ -1277,7 +1305,10 @@
       </c>
       <c r="P14" s="2">
         <f t="shared" si="1"/>
-        <v>370.18700000000001</v>
+        <v>414.262</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>15.738</v>
       </c>
       <c r="R14" s="15"/>
     </row>
@@ -1327,7 +1358,10 @@
       </c>
       <c r="P15" s="2">
         <f t="shared" si="1"/>
-        <v>52.753999999999998</v>
+        <v>60.0015</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>4.9984999999999999</v>
       </c>
       <c r="R15" s="15"/>
     </row>
@@ -1377,7 +1411,10 @@
       </c>
       <c r="P16" s="2">
         <f t="shared" si="1"/>
-        <v>13.398000000000001</v>
+        <v>15.003999999999991</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>204.99600000000001</v>
       </c>
       <c r="R16" s="15"/>
     </row>
@@ -1429,6 +1466,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="Q17" s="2">
+        <v>60</v>
+      </c>
       <c r="R17" s="15"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.35">
@@ -1477,7 +1517,10 @@
       </c>
       <c r="P18" s="2">
         <f t="shared" si="1"/>
-        <v>3.2160000000000002</v>
+        <v>3.5999999999999943</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>116.4</v>
       </c>
       <c r="R18" s="15"/>
     </row>
@@ -1529,6 +1572,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="Q19" s="2">
+        <v>50</v>
+      </c>
       <c r="R19" s="15"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
@@ -1577,7 +1623,10 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" si="1"/>
-        <v>40.199999999999996</v>
+        <v>45.024000000000001</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>624.976</v>
       </c>
       <c r="R20" s="15"/>
     </row>
@@ -1603,6 +1652,7 @@
       <c r="N21" s="8"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
       <c r="R21" s="15"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
@@ -1651,7 +1701,10 @@
       </c>
       <c r="P22" s="2">
         <f t="shared" si="1"/>
-        <v>135.53900000000002</v>
+        <v>151.50099999999998</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>78.499000000000024</v>
       </c>
       <c r="R22" s="15"/>
     </row>
@@ -1701,7 +1754,10 @@
       </c>
       <c r="P23" s="2">
         <f t="shared" si="1"/>
-        <v>376.53</v>
+        <v>420.94499999999999</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>104.05500000000001</v>
       </c>
       <c r="R23" s="15"/>
     </row>
@@ -1751,7 +1807,10 @@
       </c>
       <c r="P24" s="2">
         <f t="shared" si="1"/>
-        <v>644.10670000000005</v>
+        <v>719.96699999999998</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>23.033000000000015</v>
       </c>
       <c r="R24" s="15"/>
     </row>
@@ -1777,6 +1836,7 @@
       <c r="N25" s="8"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
       <c r="R25" s="15"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.35">
@@ -1825,7 +1885,10 @@
       </c>
       <c r="P26" s="2">
         <f t="shared" si="1"/>
-        <v>1061.2859999999998</v>
+        <v>1390.4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>189.59999999999991</v>
       </c>
       <c r="R26" s="15"/>
     </row>
@@ -1851,6 +1914,7 @@
       <c r="N27" s="8"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
       <c r="R27" s="15"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
@@ -1899,7 +1963,10 @@
       </c>
       <c r="P28" s="2">
         <f t="shared" si="1"/>
-        <v>191.7835</v>
+        <v>213.99099999999999</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>21.009000000000015</v>
       </c>
       <c r="R28" s="15"/>
     </row>
@@ -1949,7 +2016,10 @@
       </c>
       <c r="P29" s="2">
         <f t="shared" si="1"/>
-        <v>138.006</v>
+        <v>153.99600000000001</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>51.003999999999991</v>
       </c>
       <c r="R29" s="15"/>
     </row>
@@ -1975,6 +2045,7 @@
       <c r="N30" s="8"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
       <c r="R30" s="15"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
@@ -2023,7 +2094,10 @@
       </c>
       <c r="P31" s="2">
         <f t="shared" si="1"/>
-        <v>1530.048</v>
+        <v>1809.6</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>110.40000000000009</v>
       </c>
       <c r="R31" s="15"/>
     </row>
@@ -2075,6 +2149,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="Q32" s="2">
+        <v>190</v>
+      </c>
       <c r="R32" s="15"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.35">
@@ -2124,6 +2201,9 @@
       <c r="P33" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>890</v>
       </c>
       <c r="R33" s="15"/>
     </row>
@@ -2149,6 +2229,7 @@
       <c r="N34" s="8"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
       <c r="R34" s="15"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.35">
@@ -2197,7 +2278,10 @@
       </c>
       <c r="P35" s="2">
         <f t="shared" si="1"/>
-        <v>282.036</v>
+        <v>314.697</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>255.303</v>
       </c>
       <c r="R35" s="15"/>
     </row>
@@ -2247,7 +2331,10 @@
       </c>
       <c r="P36" s="2">
         <f t="shared" si="1"/>
-        <v>21.51</v>
+        <v>24</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>26</v>
       </c>
       <c r="R36" s="15"/>
     </row>
@@ -2297,7 +2384,10 @@
       </c>
       <c r="P37" s="2">
         <f t="shared" si="1"/>
-        <v>214.65599999999998</v>
+        <v>239.51000000000002</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>190.48999999999998</v>
       </c>
       <c r="R37" s="15"/>
     </row>
@@ -2347,7 +2437,10 @@
       </c>
       <c r="P38" s="2">
         <f t="shared" si="1"/>
-        <v>107.114</v>
+        <v>136.346</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>3.6539999999999964</v>
       </c>
       <c r="R38" s="15"/>
     </row>
@@ -2397,7 +2490,10 @@
       </c>
       <c r="P39" s="2">
         <f t="shared" si="1"/>
-        <v>39.653999999999996</v>
+        <v>45</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>135</v>
       </c>
       <c r="R39" s="15"/>
     </row>
@@ -2447,7 +2543,10 @@
       </c>
       <c r="P40" s="2">
         <f t="shared" si="1"/>
-        <v>4.7423999999999999</v>
+        <v>7.4935999999999865</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>144.50640000000001</v>
       </c>
       <c r="R40" s="15"/>
     </row>
@@ -2497,7 +2596,10 @@
       </c>
       <c r="P41" s="2">
         <f t="shared" si="1"/>
-        <v>474.54399999999998</v>
+        <v>543.24799999999993</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>64.752000000000066</v>
       </c>
       <c r="R41" s="15"/>
     </row>
@@ -2547,7 +2649,10 @@
       </c>
       <c r="P42" s="2">
         <f t="shared" si="1"/>
-        <v>26.889999999999997</v>
+        <v>30</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>70</v>
       </c>
       <c r="R42" s="15"/>
     </row>
@@ -2597,7 +2702,10 @@
       </c>
       <c r="P43" s="2">
         <f t="shared" si="1"/>
-        <v>43.498799999999996</v>
+        <v>59.993499999999983</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>221.00650000000002</v>
       </c>
       <c r="R43" s="15"/>
     </row>
@@ -2647,7 +2755,10 @@
       </c>
       <c r="P44" s="2">
         <f t="shared" si="1"/>
-        <v>150.31559999999999</v>
+        <v>220.27510000000001</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>8.724899999999991</v>
       </c>
       <c r="R44" s="15"/>
     </row>
@@ -2697,7 +2808,10 @@
       </c>
       <c r="P45" s="2">
         <f t="shared" si="1"/>
-        <v>98.350200000000001</v>
+        <v>111.14999999999999</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>5.8500000000000085</v>
       </c>
       <c r="R45" s="15"/>
     </row>
@@ -2747,7 +2861,10 @@
       </c>
       <c r="P46" s="2">
         <f t="shared" si="1"/>
-        <v>14.388400000000001</v>
+        <v>17.630600000000001</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>8.3693999999999988</v>
       </c>
       <c r="R46" s="15"/>
     </row>
@@ -2797,7 +2914,10 @@
       </c>
       <c r="P47" s="2">
         <f t="shared" si="1"/>
-        <v>134.24699999999999</v>
+        <v>216.81</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>2.1899999999999977</v>
       </c>
       <c r="R47" s="15"/>
     </row>
@@ -2849,55 +2969,64 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="Q48" s="2">
+        <v>18</v>
+      </c>
       <c r="R48" s="15"/>
     </row>
-    <row r="50" spans="11:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K50"/>
       <c r="L50"/>
       <c r="M50"/>
       <c r="N50"/>
       <c r="O50"/>
       <c r="P50"/>
-    </row>
-    <row r="52" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="Q50"/>
+    </row>
+    <row r="52" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K52"/>
       <c r="L52"/>
       <c r="M52"/>
       <c r="N52"/>
       <c r="O52"/>
       <c r="P52"/>
-    </row>
-    <row r="53" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="Q52"/>
+    </row>
+    <row r="53" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K53"/>
       <c r="L53"/>
       <c r="M53"/>
       <c r="N53"/>
       <c r="O53"/>
       <c r="P53"/>
-    </row>
-    <row r="54" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="Q53"/>
+    </row>
+    <row r="54" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K54"/>
       <c r="L54"/>
       <c r="M54"/>
       <c r="N54"/>
       <c r="O54"/>
       <c r="P54"/>
-    </row>
-    <row r="55" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="Q54"/>
+    </row>
+    <row r="55" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K55"/>
       <c r="L55"/>
       <c r="M55"/>
       <c r="N55"/>
       <c r="O55"/>
       <c r="P55"/>
-    </row>
-    <row r="56" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="Q55"/>
+    </row>
+    <row r="56" spans="11:17" x14ac:dyDescent="0.35">
       <c r="K56"/>
       <c r="L56"/>
       <c r="M56"/>
       <c r="N56"/>
       <c r="O56"/>
       <c r="P56"/>
+      <c r="Q56"/>
     </row>
   </sheetData>
   <autoFilter ref="C2:O48" xr:uid="{40A1E5AA-D824-4563-8855-5A2BA24ADD2B}"/>

</xml_diff>